<commit_message>
feat(CustomerLead): import data old
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/template-data-marketing.xlsx
+++ b/src/storage/app/excel-exporter/templates/template-data-marketing.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Họ Và Tên</t>
   </si>
@@ -38,7 +38,13 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
+    <t xml:space="preserve">Facebook</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nguồn tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghi chú</t>
   </si>
   <si>
     <t xml:space="preserve">Nguyễn Văn Đáng</t>
@@ -252,24 +258,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="21.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="11" style="0" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -291,3024 +297,3031 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F173" s="4"/>
+      <c r="G173" s="4"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F175" s="4"/>
+      <c r="G175" s="4"/>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F183" s="4"/>
+      <c r="G183" s="4"/>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F185" s="4"/>
+      <c r="G185" s="4"/>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F186" s="4"/>
+      <c r="G186" s="4"/>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F187" s="4"/>
+      <c r="G187" s="4"/>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F188" s="4"/>
+      <c r="G188" s="4"/>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F189" s="4"/>
+      <c r="G189" s="4"/>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F190" s="4"/>
+      <c r="G190" s="4"/>
     </row>
     <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F191" s="4"/>
+      <c r="G191" s="4"/>
     </row>
     <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F192" s="4"/>
+      <c r="G192" s="4"/>
     </row>
     <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F193" s="4"/>
+      <c r="G193" s="4"/>
     </row>
     <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F194" s="4"/>
+      <c r="G194" s="4"/>
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F195" s="4"/>
+      <c r="G195" s="4"/>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F196" s="4"/>
+      <c r="G196" s="4"/>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F197" s="4"/>
+      <c r="G197" s="4"/>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F198" s="4"/>
+      <c r="G198" s="4"/>
     </row>
     <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F199" s="4"/>
+      <c r="G199" s="4"/>
     </row>
     <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F200" s="4"/>
+      <c r="G200" s="4"/>
     </row>
     <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F201" s="4"/>
+      <c r="G201" s="4"/>
     </row>
     <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F202" s="4"/>
+      <c r="G202" s="4"/>
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F203" s="4"/>
+      <c r="G203" s="4"/>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F204" s="4"/>
+      <c r="G204" s="4"/>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F205" s="4"/>
+      <c r="G205" s="4"/>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F206" s="4"/>
+      <c r="G206" s="4"/>
     </row>
     <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F207" s="4"/>
+      <c r="G207" s="4"/>
     </row>
     <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F208" s="4"/>
+      <c r="G208" s="4"/>
     </row>
     <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F209" s="4"/>
+      <c r="G209" s="4"/>
     </row>
     <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F210" s="4"/>
+      <c r="G210" s="4"/>
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F211" s="4"/>
+      <c r="G211" s="4"/>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F212" s="4"/>
+      <c r="G212" s="4"/>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F213" s="4"/>
+      <c r="G213" s="4"/>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F214" s="4"/>
+      <c r="G214" s="4"/>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F215" s="4"/>
+      <c r="G215" s="4"/>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F216" s="4"/>
+      <c r="G216" s="4"/>
     </row>
     <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F217" s="4"/>
+      <c r="G217" s="4"/>
     </row>
     <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F218" s="4"/>
+      <c r="G218" s="4"/>
     </row>
     <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F219" s="4"/>
+      <c r="G219" s="4"/>
     </row>
     <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F220" s="4"/>
+      <c r="G220" s="4"/>
     </row>
     <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F221" s="4"/>
+      <c r="G221" s="4"/>
     </row>
     <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F222" s="4"/>
+      <c r="G222" s="4"/>
     </row>
     <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F223" s="4"/>
+      <c r="G223" s="4"/>
     </row>
     <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F224" s="4"/>
+      <c r="G224" s="4"/>
     </row>
     <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F225" s="4"/>
+      <c r="G225" s="4"/>
     </row>
     <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F226" s="4"/>
+      <c r="G226" s="4"/>
     </row>
     <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F227" s="4"/>
+      <c r="G227" s="4"/>
     </row>
     <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F228" s="4"/>
+      <c r="G228" s="4"/>
     </row>
     <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F229" s="4"/>
+      <c r="G229" s="4"/>
     </row>
     <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F230" s="4"/>
+      <c r="G230" s="4"/>
     </row>
     <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F231" s="4"/>
+      <c r="G231" s="4"/>
     </row>
     <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F232" s="4"/>
+      <c r="G232" s="4"/>
     </row>
     <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F233" s="4"/>
+      <c r="G233" s="4"/>
     </row>
     <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F234" s="4"/>
+      <c r="G234" s="4"/>
     </row>
     <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F235" s="4"/>
+      <c r="G235" s="4"/>
     </row>
     <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F236" s="4"/>
+      <c r="G236" s="4"/>
     </row>
     <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F237" s="4"/>
+      <c r="G237" s="4"/>
     </row>
     <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F238" s="4"/>
+      <c r="G238" s="4"/>
     </row>
     <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F239" s="4"/>
+      <c r="G239" s="4"/>
     </row>
     <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F240" s="4"/>
+      <c r="G240" s="4"/>
     </row>
     <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F241" s="4"/>
+      <c r="G241" s="4"/>
     </row>
     <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F242" s="4"/>
+      <c r="G242" s="4"/>
     </row>
     <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F243" s="4"/>
+      <c r="G243" s="4"/>
     </row>
     <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F244" s="4"/>
+      <c r="G244" s="4"/>
     </row>
     <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F245" s="4"/>
+      <c r="G245" s="4"/>
     </row>
     <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F246" s="4"/>
+      <c r="G246" s="4"/>
     </row>
     <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F247" s="4"/>
+      <c r="G247" s="4"/>
     </row>
     <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F248" s="4"/>
+      <c r="G248" s="4"/>
     </row>
     <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F249" s="4"/>
+      <c r="G249" s="4"/>
     </row>
     <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F250" s="4"/>
+      <c r="G250" s="4"/>
     </row>
     <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F251" s="4"/>
+      <c r="G251" s="4"/>
     </row>
     <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F252" s="4"/>
+      <c r="G252" s="4"/>
     </row>
     <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F253" s="4"/>
+      <c r="G253" s="4"/>
     </row>
     <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F254" s="4"/>
+      <c r="G254" s="4"/>
     </row>
     <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F255" s="4"/>
+      <c r="G255" s="4"/>
     </row>
     <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F256" s="4"/>
+      <c r="G256" s="4"/>
     </row>
     <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F257" s="4"/>
+      <c r="G257" s="4"/>
     </row>
     <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F258" s="4"/>
+      <c r="G258" s="4"/>
     </row>
     <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F259" s="4"/>
+      <c r="G259" s="4"/>
     </row>
     <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F260" s="4"/>
+      <c r="G260" s="4"/>
     </row>
     <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F261" s="4"/>
+      <c r="G261" s="4"/>
     </row>
     <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F262" s="4"/>
+      <c r="G262" s="4"/>
     </row>
     <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F263" s="4"/>
+      <c r="G263" s="4"/>
     </row>
     <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F264" s="4"/>
+      <c r="G264" s="4"/>
     </row>
     <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F265" s="4"/>
+      <c r="G265" s="4"/>
     </row>
     <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F266" s="4"/>
+      <c r="G266" s="4"/>
     </row>
     <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F267" s="4"/>
+      <c r="G267" s="4"/>
     </row>
     <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F268" s="4"/>
+      <c r="G268" s="4"/>
     </row>
     <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F269" s="4"/>
+      <c r="G269" s="4"/>
     </row>
     <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F270" s="4"/>
+      <c r="G270" s="4"/>
     </row>
     <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F271" s="4"/>
+      <c r="G271" s="4"/>
     </row>
     <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F272" s="4"/>
+      <c r="G272" s="4"/>
     </row>
     <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F273" s="4"/>
+      <c r="G273" s="4"/>
     </row>
     <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F274" s="4"/>
+      <c r="G274" s="4"/>
     </row>
     <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F275" s="4"/>
+      <c r="G275" s="4"/>
     </row>
     <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F276" s="4"/>
+      <c r="G276" s="4"/>
     </row>
     <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F277" s="4"/>
+      <c r="G277" s="4"/>
     </row>
     <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F278" s="4"/>
+      <c r="G278" s="4"/>
     </row>
     <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F279" s="4"/>
+      <c r="G279" s="4"/>
     </row>
     <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F280" s="4"/>
+      <c r="G280" s="4"/>
     </row>
     <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F281" s="4"/>
+      <c r="G281" s="4"/>
     </row>
     <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F282" s="4"/>
+      <c r="G282" s="4"/>
     </row>
     <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F283" s="4"/>
+      <c r="G283" s="4"/>
     </row>
     <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F284" s="4"/>
+      <c r="G284" s="4"/>
     </row>
     <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F285" s="4"/>
+      <c r="G285" s="4"/>
     </row>
     <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F286" s="4"/>
+      <c r="G286" s="4"/>
     </row>
     <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F287" s="4"/>
+      <c r="G287" s="4"/>
     </row>
     <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F288" s="4"/>
+      <c r="G288" s="4"/>
     </row>
     <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F289" s="4"/>
+      <c r="G289" s="4"/>
     </row>
     <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F290" s="4"/>
+      <c r="G290" s="4"/>
     </row>
     <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F291" s="4"/>
+      <c r="G291" s="4"/>
     </row>
     <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F292" s="4"/>
+      <c r="G292" s="4"/>
     </row>
     <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F293" s="4"/>
+      <c r="G293" s="4"/>
     </row>
     <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F294" s="4"/>
+      <c r="G294" s="4"/>
     </row>
     <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F295" s="4"/>
+      <c r="G295" s="4"/>
     </row>
     <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F296" s="4"/>
+      <c r="G296" s="4"/>
     </row>
     <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F297" s="4"/>
+      <c r="G297" s="4"/>
     </row>
     <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F298" s="4"/>
+      <c r="G298" s="4"/>
     </row>
     <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F299" s="4"/>
+      <c r="G299" s="4"/>
     </row>
     <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F300" s="4"/>
+      <c r="G300" s="4"/>
     </row>
     <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F301" s="4"/>
+      <c r="G301" s="4"/>
     </row>
     <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F302" s="4"/>
+      <c r="G302" s="4"/>
     </row>
     <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F303" s="4"/>
+      <c r="G303" s="4"/>
     </row>
     <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F304" s="4"/>
+      <c r="G304" s="4"/>
     </row>
     <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F305" s="4"/>
+      <c r="G305" s="4"/>
     </row>
     <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F306" s="4"/>
+      <c r="G306" s="4"/>
     </row>
     <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F307" s="4"/>
+      <c r="G307" s="4"/>
     </row>
     <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F308" s="4"/>
+      <c r="G308" s="4"/>
     </row>
     <row r="309" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F309" s="4"/>
+      <c r="G309" s="4"/>
     </row>
     <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F310" s="4"/>
+      <c r="G310" s="4"/>
     </row>
     <row r="311" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F311" s="4"/>
+      <c r="G311" s="4"/>
     </row>
     <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F312" s="4"/>
+      <c r="G312" s="4"/>
     </row>
     <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F313" s="4"/>
+      <c r="G313" s="4"/>
     </row>
     <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F314" s="4"/>
+      <c r="G314" s="4"/>
     </row>
     <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F315" s="4"/>
+      <c r="G315" s="4"/>
     </row>
     <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F316" s="4"/>
+      <c r="G316" s="4"/>
     </row>
     <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F317" s="4"/>
+      <c r="G317" s="4"/>
     </row>
     <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F318" s="4"/>
+      <c r="G318" s="4"/>
     </row>
     <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F319" s="4"/>
+      <c r="G319" s="4"/>
     </row>
     <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F320" s="4"/>
+      <c r="G320" s="4"/>
     </row>
     <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F321" s="4"/>
+      <c r="G321" s="4"/>
     </row>
     <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F322" s="4"/>
+      <c r="G322" s="4"/>
     </row>
     <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F323" s="4"/>
+      <c r="G323" s="4"/>
     </row>
     <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F324" s="4"/>
+      <c r="G324" s="4"/>
     </row>
     <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F325" s="4"/>
+      <c r="G325" s="4"/>
     </row>
     <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F326" s="4"/>
+      <c r="G326" s="4"/>
     </row>
     <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F327" s="4"/>
+      <c r="G327" s="4"/>
     </row>
     <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F328" s="4"/>
+      <c r="G328" s="4"/>
     </row>
     <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F329" s="4"/>
+      <c r="G329" s="4"/>
     </row>
     <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F330" s="4"/>
+      <c r="G330" s="4"/>
     </row>
     <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F331" s="4"/>
+      <c r="G331" s="4"/>
     </row>
     <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F332" s="4"/>
+      <c r="G332" s="4"/>
     </row>
     <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F333" s="4"/>
+      <c r="G333" s="4"/>
     </row>
     <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F334" s="4"/>
+      <c r="G334" s="4"/>
     </row>
     <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F335" s="4"/>
+      <c r="G335" s="4"/>
     </row>
     <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F336" s="4"/>
+      <c r="G336" s="4"/>
     </row>
     <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F337" s="4"/>
+      <c r="G337" s="4"/>
     </row>
     <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F338" s="4"/>
+      <c r="G338" s="4"/>
     </row>
     <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F339" s="4"/>
+      <c r="G339" s="4"/>
     </row>
     <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F340" s="4"/>
+      <c r="G340" s="4"/>
     </row>
     <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F341" s="4"/>
+      <c r="G341" s="4"/>
     </row>
     <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F342" s="4"/>
+      <c r="G342" s="4"/>
     </row>
     <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F343" s="4"/>
+      <c r="G343" s="4"/>
     </row>
     <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F344" s="4"/>
+      <c r="G344" s="4"/>
     </row>
     <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F345" s="4"/>
+      <c r="G345" s="4"/>
     </row>
     <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F346" s="4"/>
+      <c r="G346" s="4"/>
     </row>
     <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F347" s="4"/>
+      <c r="G347" s="4"/>
     </row>
     <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F348" s="4"/>
+      <c r="G348" s="4"/>
     </row>
     <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F349" s="4"/>
+      <c r="G349" s="4"/>
     </row>
     <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F350" s="4"/>
+      <c r="G350" s="4"/>
     </row>
     <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F351" s="4"/>
+      <c r="G351" s="4"/>
     </row>
     <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F352" s="4"/>
+      <c r="G352" s="4"/>
     </row>
     <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F353" s="4"/>
+      <c r="G353" s="4"/>
     </row>
     <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F354" s="4"/>
+      <c r="G354" s="4"/>
     </row>
     <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F355" s="4"/>
+      <c r="G355" s="4"/>
     </row>
     <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F356" s="4"/>
+      <c r="G356" s="4"/>
     </row>
     <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F357" s="4"/>
+      <c r="G357" s="4"/>
     </row>
     <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F358" s="4"/>
+      <c r="G358" s="4"/>
     </row>
     <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F359" s="4"/>
+      <c r="G359" s="4"/>
     </row>
     <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F360" s="4"/>
+      <c r="G360" s="4"/>
     </row>
     <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F361" s="4"/>
+      <c r="G361" s="4"/>
     </row>
     <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F362" s="4"/>
+      <c r="G362" s="4"/>
     </row>
     <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F363" s="4"/>
+      <c r="G363" s="4"/>
     </row>
     <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F364" s="4"/>
+      <c r="G364" s="4"/>
     </row>
     <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F365" s="4"/>
+      <c r="G365" s="4"/>
     </row>
     <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F366" s="4"/>
+      <c r="G366" s="4"/>
     </row>
     <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F367" s="4"/>
+      <c r="G367" s="4"/>
     </row>
     <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F368" s="4"/>
+      <c r="G368" s="4"/>
     </row>
     <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F369" s="4"/>
+      <c r="G369" s="4"/>
     </row>
     <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F370" s="4"/>
+      <c r="G370" s="4"/>
     </row>
     <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F371" s="4"/>
+      <c r="G371" s="4"/>
     </row>
     <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F372" s="4"/>
+      <c r="G372" s="4"/>
     </row>
     <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F373" s="4"/>
+      <c r="G373" s="4"/>
     </row>
     <row r="374" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F374" s="4"/>
+      <c r="G374" s="4"/>
     </row>
     <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F375" s="4"/>
+      <c r="G375" s="4"/>
     </row>
     <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F376" s="4"/>
+      <c r="G376" s="4"/>
     </row>
     <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F377" s="4"/>
+      <c r="G377" s="4"/>
     </row>
     <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F378" s="4"/>
+      <c r="G378" s="4"/>
     </row>
     <row r="379" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F379" s="4"/>
+      <c r="G379" s="4"/>
     </row>
     <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F380" s="4"/>
+      <c r="G380" s="4"/>
     </row>
     <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F381" s="4"/>
+      <c r="G381" s="4"/>
     </row>
     <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F382" s="4"/>
+      <c r="G382" s="4"/>
     </row>
     <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F383" s="4"/>
+      <c r="G383" s="4"/>
     </row>
     <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F384" s="4"/>
+      <c r="G384" s="4"/>
     </row>
     <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F385" s="4"/>
+      <c r="G385" s="4"/>
     </row>
     <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F386" s="4"/>
+      <c r="G386" s="4"/>
     </row>
     <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F387" s="4"/>
+      <c r="G387" s="4"/>
     </row>
     <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F388" s="4"/>
+      <c r="G388" s="4"/>
     </row>
     <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F389" s="4"/>
+      <c r="G389" s="4"/>
     </row>
     <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F390" s="4"/>
+      <c r="G390" s="4"/>
     </row>
     <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F391" s="4"/>
+      <c r="G391" s="4"/>
     </row>
     <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F392" s="4"/>
+      <c r="G392" s="4"/>
     </row>
     <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F393" s="4"/>
+      <c r="G393" s="4"/>
     </row>
     <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F394" s="4"/>
+      <c r="G394" s="4"/>
     </row>
     <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F395" s="4"/>
+      <c r="G395" s="4"/>
     </row>
     <row r="396" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F396" s="4"/>
+      <c r="G396" s="4"/>
     </row>
     <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F397" s="4"/>
+      <c r="G397" s="4"/>
     </row>
     <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F398" s="4"/>
+      <c r="G398" s="4"/>
     </row>
     <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F399" s="4"/>
+      <c r="G399" s="4"/>
     </row>
     <row r="400" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F400" s="4"/>
+      <c r="G400" s="4"/>
     </row>
     <row r="401" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F401" s="4"/>
+      <c r="G401" s="4"/>
     </row>
     <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F402" s="4"/>
+      <c r="G402" s="4"/>
     </row>
     <row r="403" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F403" s="4"/>
+      <c r="G403" s="4"/>
     </row>
     <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F404" s="4"/>
+      <c r="G404" s="4"/>
     </row>
     <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F405" s="4"/>
+      <c r="G405" s="4"/>
     </row>
     <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F406" s="4"/>
+      <c r="G406" s="4"/>
     </row>
     <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F407" s="4"/>
+      <c r="G407" s="4"/>
     </row>
     <row r="408" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F408" s="4"/>
+      <c r="G408" s="4"/>
     </row>
     <row r="409" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F409" s="4"/>
+      <c r="G409" s="4"/>
     </row>
     <row r="410" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F410" s="4"/>
+      <c r="G410" s="4"/>
     </row>
     <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F411" s="4"/>
+      <c r="G411" s="4"/>
     </row>
     <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F412" s="4"/>
+      <c r="G412" s="4"/>
     </row>
     <row r="413" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F413" s="4"/>
+      <c r="G413" s="4"/>
     </row>
     <row r="414" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F414" s="4"/>
+      <c r="G414" s="4"/>
     </row>
     <row r="415" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F415" s="4"/>
+      <c r="G415" s="4"/>
     </row>
     <row r="416" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F416" s="4"/>
+      <c r="G416" s="4"/>
     </row>
     <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F417" s="4"/>
+      <c r="G417" s="4"/>
     </row>
     <row r="418" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F418" s="4"/>
+      <c r="G418" s="4"/>
     </row>
     <row r="419" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F419" s="4"/>
+      <c r="G419" s="4"/>
     </row>
     <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F420" s="4"/>
+      <c r="G420" s="4"/>
     </row>
     <row r="421" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F421" s="4"/>
+      <c r="G421" s="4"/>
     </row>
     <row r="422" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F422" s="4"/>
+      <c r="G422" s="4"/>
     </row>
     <row r="423" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F423" s="4"/>
+      <c r="G423" s="4"/>
     </row>
     <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F424" s="4"/>
+      <c r="G424" s="4"/>
     </row>
     <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F425" s="4"/>
+      <c r="G425" s="4"/>
     </row>
     <row r="426" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F426" s="4"/>
+      <c r="G426" s="4"/>
     </row>
     <row r="427" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F427" s="4"/>
+      <c r="G427" s="4"/>
     </row>
     <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F428" s="4"/>
+      <c r="G428" s="4"/>
     </row>
     <row r="429" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F429" s="4"/>
+      <c r="G429" s="4"/>
     </row>
     <row r="430" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F430" s="4"/>
+      <c r="G430" s="4"/>
     </row>
     <row r="431" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F431" s="4"/>
+      <c r="G431" s="4"/>
     </row>
     <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F432" s="4"/>
+      <c r="G432" s="4"/>
     </row>
     <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F433" s="4"/>
+      <c r="G433" s="4"/>
     </row>
     <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F434" s="4"/>
+      <c r="G434" s="4"/>
     </row>
     <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F435" s="4"/>
+      <c r="G435" s="4"/>
     </row>
     <row r="436" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F436" s="4"/>
+      <c r="G436" s="4"/>
     </row>
     <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F437" s="4"/>
+      <c r="G437" s="4"/>
     </row>
     <row r="438" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F438" s="4"/>
+      <c r="G438" s="4"/>
     </row>
     <row r="439" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F439" s="4"/>
+      <c r="G439" s="4"/>
     </row>
     <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F440" s="4"/>
+      <c r="G440" s="4"/>
     </row>
     <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F441" s="4"/>
+      <c r="G441" s="4"/>
     </row>
     <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F442" s="4"/>
+      <c r="G442" s="4"/>
     </row>
     <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F443" s="4"/>
+      <c r="G443" s="4"/>
     </row>
     <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F444" s="4"/>
+      <c r="G444" s="4"/>
     </row>
     <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F445" s="4"/>
+      <c r="G445" s="4"/>
     </row>
     <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F446" s="4"/>
+      <c r="G446" s="4"/>
     </row>
     <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F447" s="4"/>
+      <c r="G447" s="4"/>
     </row>
     <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F448" s="4"/>
+      <c r="G448" s="4"/>
     </row>
     <row r="449" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F449" s="4"/>
+      <c r="G449" s="4"/>
     </row>
     <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F450" s="4"/>
+      <c r="G450" s="4"/>
     </row>
     <row r="451" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F451" s="4"/>
+      <c r="G451" s="4"/>
     </row>
     <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F452" s="4"/>
+      <c r="G452" s="4"/>
     </row>
     <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F453" s="4"/>
+      <c r="G453" s="4"/>
     </row>
     <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F454" s="4"/>
+      <c r="G454" s="4"/>
     </row>
     <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F455" s="4"/>
+      <c r="G455" s="4"/>
     </row>
     <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F456" s="4"/>
+      <c r="G456" s="4"/>
     </row>
     <row r="457" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F457" s="4"/>
+      <c r="G457" s="4"/>
     </row>
     <row r="458" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F458" s="4"/>
+      <c r="G458" s="4"/>
     </row>
     <row r="459" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F459" s="4"/>
+      <c r="G459" s="4"/>
     </row>
     <row r="460" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F460" s="4"/>
+      <c r="G460" s="4"/>
     </row>
     <row r="461" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F461" s="4"/>
+      <c r="G461" s="4"/>
     </row>
     <row r="462" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F462" s="4"/>
+      <c r="G462" s="4"/>
     </row>
     <row r="463" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F463" s="4"/>
+      <c r="G463" s="4"/>
     </row>
     <row r="464" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F464" s="4"/>
+      <c r="G464" s="4"/>
     </row>
     <row r="465" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F465" s="4"/>
+      <c r="G465" s="4"/>
     </row>
     <row r="466" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F466" s="4"/>
+      <c r="G466" s="4"/>
     </row>
     <row r="467" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F467" s="4"/>
+      <c r="G467" s="4"/>
     </row>
     <row r="468" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F468" s="4"/>
+      <c r="G468" s="4"/>
     </row>
     <row r="469" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F469" s="4"/>
+      <c r="G469" s="4"/>
     </row>
     <row r="470" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F470" s="4"/>
+      <c r="G470" s="4"/>
     </row>
     <row r="471" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F471" s="4"/>
+      <c r="G471" s="4"/>
     </row>
     <row r="472" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F472" s="4"/>
+      <c r="G472" s="4"/>
     </row>
     <row r="473" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F473" s="4"/>
+      <c r="G473" s="4"/>
     </row>
     <row r="474" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F474" s="4"/>
+      <c r="G474" s="4"/>
     </row>
     <row r="475" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F475" s="4"/>
+      <c r="G475" s="4"/>
     </row>
     <row r="476" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F476" s="4"/>
+      <c r="G476" s="4"/>
     </row>
     <row r="477" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F477" s="4"/>
+      <c r="G477" s="4"/>
     </row>
     <row r="478" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F478" s="4"/>
+      <c r="G478" s="4"/>
     </row>
     <row r="479" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F479" s="4"/>
+      <c r="G479" s="4"/>
     </row>
     <row r="480" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F480" s="4"/>
+      <c r="G480" s="4"/>
     </row>
     <row r="481" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F481" s="4"/>
+      <c r="G481" s="4"/>
     </row>
     <row r="482" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F482" s="4"/>
+      <c r="G482" s="4"/>
     </row>
     <row r="483" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F483" s="4"/>
+      <c r="G483" s="4"/>
     </row>
     <row r="484" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F484" s="4"/>
+      <c r="G484" s="4"/>
     </row>
     <row r="485" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F485" s="4"/>
+      <c r="G485" s="4"/>
     </row>
     <row r="486" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F486" s="4"/>
+      <c r="G486" s="4"/>
     </row>
     <row r="487" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F487" s="4"/>
+      <c r="G487" s="4"/>
     </row>
     <row r="488" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F488" s="4"/>
+      <c r="G488" s="4"/>
     </row>
     <row r="489" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F489" s="4"/>
+      <c r="G489" s="4"/>
     </row>
     <row r="490" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F490" s="4"/>
+      <c r="G490" s="4"/>
     </row>
     <row r="491" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F491" s="4"/>
+      <c r="G491" s="4"/>
     </row>
     <row r="492" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F492" s="4"/>
+      <c r="G492" s="4"/>
     </row>
     <row r="493" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F493" s="4"/>
+      <c r="G493" s="4"/>
     </row>
     <row r="494" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F494" s="4"/>
+      <c r="G494" s="4"/>
     </row>
     <row r="495" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F495" s="4"/>
+      <c r="G495" s="4"/>
     </row>
     <row r="496" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F496" s="4"/>
+      <c r="G496" s="4"/>
     </row>
     <row r="497" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F497" s="4"/>
+      <c r="G497" s="4"/>
     </row>
     <row r="498" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F498" s="4"/>
+      <c r="G498" s="4"/>
     </row>
     <row r="499" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F499" s="4"/>
+      <c r="G499" s="4"/>
     </row>
     <row r="500" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F500" s="4"/>
+      <c r="G500" s="4"/>
     </row>
     <row r="501" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F501" s="4"/>
+      <c r="G501" s="4"/>
     </row>
     <row r="502" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F502" s="4"/>
+      <c r="G502" s="4"/>
     </row>
     <row r="503" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F503" s="4"/>
+      <c r="G503" s="4"/>
     </row>
     <row r="504" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F504" s="4"/>
+      <c r="G504" s="4"/>
     </row>
     <row r="505" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F505" s="4"/>
+      <c r="G505" s="4"/>
     </row>
     <row r="506" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F506" s="4"/>
+      <c r="G506" s="4"/>
     </row>
     <row r="507" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F507" s="4"/>
+      <c r="G507" s="4"/>
     </row>
     <row r="508" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F508" s="4"/>
+      <c r="G508" s="4"/>
     </row>
     <row r="509" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F509" s="4"/>
+      <c r="G509" s="4"/>
     </row>
     <row r="510" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F510" s="4"/>
+      <c r="G510" s="4"/>
     </row>
     <row r="511" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F511" s="4"/>
+      <c r="G511" s="4"/>
     </row>
     <row r="512" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F512" s="4"/>
+      <c r="G512" s="4"/>
     </row>
     <row r="513" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F513" s="4"/>
+      <c r="G513" s="4"/>
     </row>
     <row r="514" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F514" s="4"/>
+      <c r="G514" s="4"/>
     </row>
     <row r="515" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F515" s="4"/>
+      <c r="G515" s="4"/>
     </row>
     <row r="516" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F516" s="4"/>
+      <c r="G516" s="4"/>
     </row>
     <row r="517" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F517" s="4"/>
+      <c r="G517" s="4"/>
     </row>
     <row r="518" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F518" s="4"/>
+      <c r="G518" s="4"/>
     </row>
     <row r="519" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F519" s="4"/>
+      <c r="G519" s="4"/>
     </row>
     <row r="520" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F520" s="4"/>
+      <c r="G520" s="4"/>
     </row>
     <row r="521" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F521" s="4"/>
+      <c r="G521" s="4"/>
     </row>
     <row r="522" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F522" s="4"/>
+      <c r="G522" s="4"/>
     </row>
     <row r="523" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F523" s="4"/>
+      <c r="G523" s="4"/>
     </row>
     <row r="524" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F524" s="4"/>
+      <c r="G524" s="4"/>
     </row>
     <row r="525" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F525" s="4"/>
+      <c r="G525" s="4"/>
     </row>
     <row r="526" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F526" s="4"/>
+      <c r="G526" s="4"/>
     </row>
     <row r="527" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F527" s="4"/>
+      <c r="G527" s="4"/>
     </row>
     <row r="528" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F528" s="4"/>
+      <c r="G528" s="4"/>
     </row>
     <row r="529" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F529" s="4"/>
+      <c r="G529" s="4"/>
     </row>
     <row r="530" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F530" s="4"/>
+      <c r="G530" s="4"/>
     </row>
     <row r="531" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F531" s="4"/>
+      <c r="G531" s="4"/>
     </row>
     <row r="532" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F532" s="4"/>
+      <c r="G532" s="4"/>
     </row>
     <row r="533" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F533" s="4"/>
+      <c r="G533" s="4"/>
     </row>
     <row r="534" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F534" s="4"/>
+      <c r="G534" s="4"/>
     </row>
     <row r="535" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F535" s="4"/>
+      <c r="G535" s="4"/>
     </row>
     <row r="536" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F536" s="4"/>
+      <c r="G536" s="4"/>
     </row>
     <row r="537" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F537" s="4"/>
+      <c r="G537" s="4"/>
     </row>
     <row r="538" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F538" s="4"/>
+      <c r="G538" s="4"/>
     </row>
     <row r="539" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F539" s="4"/>
+      <c r="G539" s="4"/>
     </row>
     <row r="540" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F540" s="4"/>
+      <c r="G540" s="4"/>
     </row>
     <row r="541" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F541" s="4"/>
+      <c r="G541" s="4"/>
     </row>
     <row r="542" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F542" s="4"/>
+      <c r="G542" s="4"/>
     </row>
     <row r="543" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F543" s="4"/>
+      <c r="G543" s="4"/>
     </row>
     <row r="544" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F544" s="4"/>
+      <c r="G544" s="4"/>
     </row>
     <row r="545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F545" s="4"/>
+      <c r="G545" s="4"/>
     </row>
     <row r="546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F546" s="4"/>
+      <c r="G546" s="4"/>
     </row>
     <row r="547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F547" s="4"/>
+      <c r="G547" s="4"/>
     </row>
     <row r="548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F548" s="4"/>
+      <c r="G548" s="4"/>
     </row>
     <row r="549" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F549" s="4"/>
+      <c r="G549" s="4"/>
     </row>
     <row r="550" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F550" s="4"/>
+      <c r="G550" s="4"/>
     </row>
     <row r="551" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F551" s="4"/>
+      <c r="G551" s="4"/>
     </row>
     <row r="552" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F552" s="4"/>
+      <c r="G552" s="4"/>
     </row>
     <row r="553" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F553" s="4"/>
+      <c r="G553" s="4"/>
     </row>
     <row r="554" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F554" s="4"/>
+      <c r="G554" s="4"/>
     </row>
     <row r="555" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F555" s="4"/>
+      <c r="G555" s="4"/>
     </row>
     <row r="556" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F556" s="4"/>
+      <c r="G556" s="4"/>
     </row>
     <row r="557" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F557" s="4"/>
+      <c r="G557" s="4"/>
     </row>
     <row r="558" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F558" s="4"/>
+      <c r="G558" s="4"/>
     </row>
     <row r="559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F559" s="4"/>
+      <c r="G559" s="4"/>
     </row>
     <row r="560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F560" s="4"/>
+      <c r="G560" s="4"/>
     </row>
     <row r="561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F561" s="4"/>
+      <c r="G561" s="4"/>
     </row>
     <row r="562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F562" s="4"/>
+      <c r="G562" s="4"/>
     </row>
     <row r="563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F563" s="4"/>
+      <c r="G563" s="4"/>
     </row>
     <row r="564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F564" s="4"/>
+      <c r="G564" s="4"/>
     </row>
     <row r="565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F565" s="4"/>
+      <c r="G565" s="4"/>
     </row>
     <row r="566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F566" s="4"/>
+      <c r="G566" s="4"/>
     </row>
     <row r="567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F567" s="4"/>
+      <c r="G567" s="4"/>
     </row>
     <row r="568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F568" s="4"/>
+      <c r="G568" s="4"/>
     </row>
     <row r="569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F569" s="4"/>
+      <c r="G569" s="4"/>
     </row>
     <row r="570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F570" s="4"/>
+      <c r="G570" s="4"/>
     </row>
     <row r="571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F571" s="4"/>
+      <c r="G571" s="4"/>
     </row>
     <row r="572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F572" s="4"/>
+      <c r="G572" s="4"/>
     </row>
     <row r="573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F573" s="4"/>
+      <c r="G573" s="4"/>
     </row>
     <row r="574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F574" s="4"/>
+      <c r="G574" s="4"/>
     </row>
     <row r="575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F575" s="4"/>
+      <c r="G575" s="4"/>
     </row>
     <row r="576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F576" s="4"/>
+      <c r="G576" s="4"/>
     </row>
     <row r="577" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F577" s="4"/>
+      <c r="G577" s="4"/>
     </row>
     <row r="578" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F578" s="4"/>
+      <c r="G578" s="4"/>
     </row>
     <row r="579" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F579" s="4"/>
+      <c r="G579" s="4"/>
     </row>
     <row r="580" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F580" s="4"/>
+      <c r="G580" s="4"/>
     </row>
     <row r="581" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F581" s="4"/>
+      <c r="G581" s="4"/>
     </row>
     <row r="582" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F582" s="4"/>
+      <c r="G582" s="4"/>
     </row>
     <row r="583" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F583" s="4"/>
+      <c r="G583" s="4"/>
     </row>
     <row r="584" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F584" s="4"/>
+      <c r="G584" s="4"/>
     </row>
     <row r="585" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F585" s="4"/>
+      <c r="G585" s="4"/>
     </row>
     <row r="586" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F586" s="4"/>
+      <c r="G586" s="4"/>
     </row>
     <row r="587" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F587" s="4"/>
+      <c r="G587" s="4"/>
     </row>
     <row r="588" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F588" s="4"/>
+      <c r="G588" s="4"/>
     </row>
     <row r="589" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F589" s="4"/>
+      <c r="G589" s="4"/>
     </row>
     <row r="590" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F590" s="4"/>
+      <c r="G590" s="4"/>
     </row>
     <row r="591" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F591" s="4"/>
+      <c r="G591" s="4"/>
     </row>
     <row r="592" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F592" s="4"/>
+      <c r="G592" s="4"/>
     </row>
     <row r="593" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F593" s="4"/>
+      <c r="G593" s="4"/>
     </row>
     <row r="594" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F594" s="4"/>
+      <c r="G594" s="4"/>
     </row>
     <row r="595" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F595" s="4"/>
+      <c r="G595" s="4"/>
     </row>
     <row r="596" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F596" s="4"/>
+      <c r="G596" s="4"/>
     </row>
     <row r="597" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F597" s="4"/>
+      <c r="G597" s="4"/>
     </row>
     <row r="598" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F598" s="4"/>
+      <c r="G598" s="4"/>
     </row>
     <row r="599" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F599" s="4"/>
+      <c r="G599" s="4"/>
     </row>
     <row r="600" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F600" s="4"/>
+      <c r="G600" s="4"/>
     </row>
     <row r="601" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F601" s="4"/>
+      <c r="G601" s="4"/>
     </row>
     <row r="602" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F602" s="4"/>
+      <c r="G602" s="4"/>
     </row>
     <row r="603" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F603" s="4"/>
+      <c r="G603" s="4"/>
     </row>
     <row r="604" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F604" s="4"/>
+      <c r="G604" s="4"/>
     </row>
     <row r="605" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F605" s="4"/>
+      <c r="G605" s="4"/>
     </row>
     <row r="606" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F606" s="4"/>
+      <c r="G606" s="4"/>
     </row>
     <row r="607" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F607" s="4"/>
+      <c r="G607" s="4"/>
     </row>
     <row r="608" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F608" s="4"/>
+      <c r="G608" s="4"/>
     </row>
     <row r="609" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F609" s="4"/>
+      <c r="G609" s="4"/>
     </row>
     <row r="610" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F610" s="4"/>
+      <c r="G610" s="4"/>
     </row>
     <row r="611" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F611" s="4"/>
+      <c r="G611" s="4"/>
     </row>
     <row r="612" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F612" s="4"/>
+      <c r="G612" s="4"/>
     </row>
     <row r="613" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F613" s="4"/>
+      <c r="G613" s="4"/>
     </row>
     <row r="614" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F614" s="4"/>
+      <c r="G614" s="4"/>
     </row>
     <row r="615" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F615" s="4"/>
+      <c r="G615" s="4"/>
     </row>
     <row r="616" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F616" s="4"/>
+      <c r="G616" s="4"/>
     </row>
     <row r="617" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F617" s="4"/>
+      <c r="G617" s="4"/>
     </row>
     <row r="618" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F618" s="4"/>
+      <c r="G618" s="4"/>
     </row>
     <row r="619" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F619" s="4"/>
+      <c r="G619" s="4"/>
     </row>
     <row r="620" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F620" s="4"/>
+      <c r="G620" s="4"/>
     </row>
     <row r="621" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F621" s="4"/>
+      <c r="G621" s="4"/>
     </row>
     <row r="622" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F622" s="4"/>
+      <c r="G622" s="4"/>
     </row>
     <row r="623" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F623" s="4"/>
+      <c r="G623" s="4"/>
     </row>
     <row r="624" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F624" s="4"/>
+      <c r="G624" s="4"/>
     </row>
     <row r="625" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F625" s="4"/>
+      <c r="G625" s="4"/>
     </row>
     <row r="626" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F626" s="4"/>
+      <c r="G626" s="4"/>
     </row>
     <row r="627" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F627" s="4"/>
+      <c r="G627" s="4"/>
     </row>
     <row r="628" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F628" s="4"/>
+      <c r="G628" s="4"/>
     </row>
     <row r="629" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F629" s="4"/>
+      <c r="G629" s="4"/>
     </row>
     <row r="630" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F630" s="4"/>
+      <c r="G630" s="4"/>
     </row>
     <row r="631" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F631" s="4"/>
+      <c r="G631" s="4"/>
     </row>
     <row r="632" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F632" s="4"/>
+      <c r="G632" s="4"/>
     </row>
     <row r="633" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F633" s="4"/>
+      <c r="G633" s="4"/>
     </row>
     <row r="634" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F634" s="4"/>
+      <c r="G634" s="4"/>
     </row>
     <row r="635" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F635" s="4"/>
+      <c r="G635" s="4"/>
     </row>
     <row r="636" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F636" s="4"/>
+      <c r="G636" s="4"/>
     </row>
     <row r="637" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F637" s="4"/>
+      <c r="G637" s="4"/>
     </row>
     <row r="638" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F638" s="4"/>
+      <c r="G638" s="4"/>
     </row>
     <row r="639" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F639" s="4"/>
+      <c r="G639" s="4"/>
     </row>
     <row r="640" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F640" s="4"/>
+      <c r="G640" s="4"/>
     </row>
     <row r="641" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F641" s="4"/>
+      <c r="G641" s="4"/>
     </row>
     <row r="642" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F642" s="4"/>
+      <c r="G642" s="4"/>
     </row>
     <row r="643" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F643" s="4"/>
+      <c r="G643" s="4"/>
     </row>
     <row r="644" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F644" s="4"/>
+      <c r="G644" s="4"/>
     </row>
     <row r="645" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F645" s="4"/>
+      <c r="G645" s="4"/>
     </row>
     <row r="646" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F646" s="4"/>
+      <c r="G646" s="4"/>
     </row>
     <row r="647" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F647" s="4"/>
+      <c r="G647" s="4"/>
     </row>
     <row r="648" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F648" s="4"/>
+      <c r="G648" s="4"/>
     </row>
     <row r="649" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F649" s="4"/>
+      <c r="G649" s="4"/>
     </row>
     <row r="650" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F650" s="4"/>
+      <c r="G650" s="4"/>
     </row>
     <row r="651" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F651" s="4"/>
+      <c r="G651" s="4"/>
     </row>
     <row r="652" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F652" s="4"/>
+      <c r="G652" s="4"/>
     </row>
     <row r="653" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F653" s="4"/>
+      <c r="G653" s="4"/>
     </row>
     <row r="654" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F654" s="4"/>
+      <c r="G654" s="4"/>
     </row>
     <row r="655" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F655" s="4"/>
+      <c r="G655" s="4"/>
     </row>
     <row r="656" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F656" s="4"/>
+      <c r="G656" s="4"/>
     </row>
     <row r="657" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F657" s="4"/>
+      <c r="G657" s="4"/>
     </row>
     <row r="658" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F658" s="4"/>
+      <c r="G658" s="4"/>
     </row>
     <row r="659" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F659" s="4"/>
+      <c r="G659" s="4"/>
     </row>
     <row r="660" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F660" s="4"/>
+      <c r="G660" s="4"/>
     </row>
     <row r="661" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F661" s="4"/>
+      <c r="G661" s="4"/>
     </row>
     <row r="662" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F662" s="4"/>
+      <c r="G662" s="4"/>
     </row>
     <row r="663" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F663" s="4"/>
+      <c r="G663" s="4"/>
     </row>
     <row r="664" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F664" s="4"/>
+      <c r="G664" s="4"/>
     </row>
     <row r="665" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F665" s="4"/>
+      <c r="G665" s="4"/>
     </row>
     <row r="666" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F666" s="4"/>
+      <c r="G666" s="4"/>
     </row>
     <row r="667" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F667" s="4"/>
+      <c r="G667" s="4"/>
     </row>
     <row r="668" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F668" s="4"/>
+      <c r="G668" s="4"/>
     </row>
     <row r="669" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F669" s="4"/>
+      <c r="G669" s="4"/>
     </row>
     <row r="670" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F670" s="4"/>
+      <c r="G670" s="4"/>
     </row>
     <row r="671" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F671" s="4"/>
+      <c r="G671" s="4"/>
     </row>
     <row r="672" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F672" s="4"/>
+      <c r="G672" s="4"/>
     </row>
     <row r="673" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F673" s="4"/>
+      <c r="G673" s="4"/>
     </row>
     <row r="674" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F674" s="4"/>
+      <c r="G674" s="4"/>
     </row>
     <row r="675" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F675" s="4"/>
+      <c r="G675" s="4"/>
     </row>
     <row r="676" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F676" s="4"/>
+      <c r="G676" s="4"/>
     </row>
     <row r="677" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F677" s="4"/>
+      <c r="G677" s="4"/>
     </row>
     <row r="678" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F678" s="4"/>
+      <c r="G678" s="4"/>
     </row>
     <row r="679" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F679" s="4"/>
+      <c r="G679" s="4"/>
     </row>
     <row r="680" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F680" s="4"/>
+      <c r="G680" s="4"/>
     </row>
     <row r="681" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F681" s="4"/>
+      <c r="G681" s="4"/>
     </row>
     <row r="682" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F682" s="4"/>
+      <c r="G682" s="4"/>
     </row>
     <row r="683" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F683" s="4"/>
+      <c r="G683" s="4"/>
     </row>
     <row r="684" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F684" s="4"/>
+      <c r="G684" s="4"/>
     </row>
     <row r="685" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F685" s="4"/>
+      <c r="G685" s="4"/>
     </row>
     <row r="686" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F686" s="4"/>
+      <c r="G686" s="4"/>
     </row>
     <row r="687" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F687" s="4"/>
+      <c r="G687" s="4"/>
     </row>
     <row r="688" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F688" s="4"/>
+      <c r="G688" s="4"/>
     </row>
     <row r="689" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F689" s="4"/>
+      <c r="G689" s="4"/>
     </row>
     <row r="690" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F690" s="4"/>
+      <c r="G690" s="4"/>
     </row>
     <row r="691" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F691" s="4"/>
+      <c r="G691" s="4"/>
     </row>
     <row r="692" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F692" s="4"/>
+      <c r="G692" s="4"/>
     </row>
     <row r="693" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F693" s="4"/>
+      <c r="G693" s="4"/>
     </row>
     <row r="694" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F694" s="4"/>
+      <c r="G694" s="4"/>
     </row>
     <row r="695" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F695" s="4"/>
+      <c r="G695" s="4"/>
     </row>
     <row r="696" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F696" s="4"/>
+      <c r="G696" s="4"/>
     </row>
     <row r="697" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F697" s="4"/>
+      <c r="G697" s="4"/>
     </row>
     <row r="698" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F698" s="4"/>
+      <c r="G698" s="4"/>
     </row>
     <row r="699" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F699" s="4"/>
+      <c r="G699" s="4"/>
     </row>
     <row r="700" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F700" s="4"/>
+      <c r="G700" s="4"/>
     </row>
     <row r="701" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F701" s="4"/>
+      <c r="G701" s="4"/>
     </row>
     <row r="702" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F702" s="4"/>
+      <c r="G702" s="4"/>
     </row>
     <row r="703" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F703" s="4"/>
+      <c r="G703" s="4"/>
     </row>
     <row r="704" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F704" s="4"/>
+      <c r="G704" s="4"/>
     </row>
     <row r="705" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F705" s="4"/>
+      <c r="G705" s="4"/>
     </row>
     <row r="706" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F706" s="4"/>
+      <c r="G706" s="4"/>
     </row>
     <row r="707" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F707" s="4"/>
+      <c r="G707" s="4"/>
     </row>
     <row r="708" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F708" s="4"/>
+      <c r="G708" s="4"/>
     </row>
     <row r="709" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F709" s="4"/>
+      <c r="G709" s="4"/>
     </row>
     <row r="710" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F710" s="4"/>
+      <c r="G710" s="4"/>
     </row>
     <row r="711" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F711" s="4"/>
+      <c r="G711" s="4"/>
     </row>
     <row r="712" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F712" s="4"/>
+      <c r="G712" s="4"/>
     </row>
     <row r="713" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F713" s="4"/>
+      <c r="G713" s="4"/>
     </row>
     <row r="714" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F714" s="4"/>
+      <c r="G714" s="4"/>
     </row>
     <row r="715" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F715" s="4"/>
+      <c r="G715" s="4"/>
     </row>
     <row r="716" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F716" s="4"/>
+      <c r="G716" s="4"/>
     </row>
     <row r="717" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F717" s="4"/>
+      <c r="G717" s="4"/>
     </row>
     <row r="718" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F718" s="4"/>
+      <c r="G718" s="4"/>
     </row>
     <row r="719" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F719" s="4"/>
+      <c r="G719" s="4"/>
     </row>
     <row r="720" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F720" s="4"/>
+      <c r="G720" s="4"/>
     </row>
     <row r="721" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F721" s="4"/>
+      <c r="G721" s="4"/>
     </row>
     <row r="722" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F722" s="4"/>
+      <c r="G722" s="4"/>
     </row>
     <row r="723" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F723" s="4"/>
+      <c r="G723" s="4"/>
     </row>
     <row r="724" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F724" s="4"/>
+      <c r="G724" s="4"/>
     </row>
     <row r="725" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F725" s="4"/>
+      <c r="G725" s="4"/>
     </row>
     <row r="726" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F726" s="4"/>
+      <c r="G726" s="4"/>
     </row>
     <row r="727" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F727" s="4"/>
+      <c r="G727" s="4"/>
     </row>
     <row r="728" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F728" s="4"/>
+      <c r="G728" s="4"/>
     </row>
     <row r="729" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F729" s="4"/>
+      <c r="G729" s="4"/>
     </row>
     <row r="730" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F730" s="4"/>
+      <c r="G730" s="4"/>
     </row>
     <row r="731" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F731" s="4"/>
+      <c r="G731" s="4"/>
     </row>
     <row r="732" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F732" s="4"/>
+      <c r="G732" s="4"/>
     </row>
     <row r="733" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F733" s="4"/>
+      <c r="G733" s="4"/>
     </row>
     <row r="734" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F734" s="4"/>
+      <c r="G734" s="4"/>
     </row>
     <row r="735" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F735" s="4"/>
+      <c r="G735" s="4"/>
     </row>
     <row r="736" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F736" s="4"/>
+      <c r="G736" s="4"/>
     </row>
     <row r="737" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F737" s="4"/>
+      <c r="G737" s="4"/>
     </row>
     <row r="738" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F738" s="4"/>
+      <c r="G738" s="4"/>
     </row>
     <row r="739" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F739" s="4"/>
+      <c r="G739" s="4"/>
     </row>
     <row r="740" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F740" s="4"/>
+      <c r="G740" s="4"/>
     </row>
     <row r="741" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F741" s="4"/>
+      <c r="G741" s="4"/>
     </row>
     <row r="742" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F742" s="4"/>
+      <c r="G742" s="4"/>
     </row>
     <row r="743" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F743" s="4"/>
+      <c r="G743" s="4"/>
     </row>
     <row r="744" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F744" s="4"/>
+      <c r="G744" s="4"/>
     </row>
     <row r="745" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F745" s="4"/>
+      <c r="G745" s="4"/>
     </row>
     <row r="746" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F746" s="4"/>
+      <c r="G746" s="4"/>
     </row>
     <row r="747" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F747" s="4"/>
+      <c r="G747" s="4"/>
     </row>
     <row r="748" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F748" s="4"/>
+      <c r="G748" s="4"/>
     </row>
     <row r="749" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F749" s="4"/>
+      <c r="G749" s="4"/>
     </row>
     <row r="750" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F750" s="4"/>
+      <c r="G750" s="4"/>
     </row>
     <row r="751" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F751" s="4"/>
+      <c r="G751" s="4"/>
     </row>
     <row r="752" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F752" s="4"/>
+      <c r="G752" s="4"/>
     </row>
     <row r="753" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F753" s="4"/>
+      <c r="G753" s="4"/>
     </row>
     <row r="754" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F754" s="4"/>
+      <c r="G754" s="4"/>
     </row>
     <row r="755" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F755" s="4"/>
+      <c r="G755" s="4"/>
     </row>
     <row r="756" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F756" s="4"/>
+      <c r="G756" s="4"/>
     </row>
     <row r="757" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F757" s="4"/>
+      <c r="G757" s="4"/>
     </row>
     <row r="758" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F758" s="4"/>
+      <c r="G758" s="4"/>
     </row>
     <row r="759" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F759" s="4"/>
+      <c r="G759" s="4"/>
     </row>
     <row r="760" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F760" s="4"/>
+      <c r="G760" s="4"/>
     </row>
     <row r="761" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F761" s="4"/>
+      <c r="G761" s="4"/>
     </row>
     <row r="762" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F762" s="4"/>
+      <c r="G762" s="4"/>
     </row>
     <row r="763" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F763" s="4"/>
+      <c r="G763" s="4"/>
     </row>
     <row r="764" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F764" s="4"/>
+      <c r="G764" s="4"/>
     </row>
     <row r="765" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F765" s="4"/>
+      <c r="G765" s="4"/>
     </row>
     <row r="766" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F766" s="4"/>
+      <c r="G766" s="4"/>
     </row>
     <row r="767" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F767" s="4"/>
+      <c r="G767" s="4"/>
     </row>
     <row r="768" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F768" s="4"/>
+      <c r="G768" s="4"/>
     </row>
     <row r="769" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F769" s="4"/>
+      <c r="G769" s="4"/>
     </row>
     <row r="770" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F770" s="4"/>
+      <c r="G770" s="4"/>
     </row>
     <row r="771" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F771" s="4"/>
+      <c r="G771" s="4"/>
     </row>
     <row r="772" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F772" s="4"/>
+      <c r="G772" s="4"/>
     </row>
     <row r="773" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F773" s="4"/>
+      <c r="G773" s="4"/>
     </row>
     <row r="774" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F774" s="4"/>
+      <c r="G774" s="4"/>
     </row>
     <row r="775" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F775" s="4"/>
+      <c r="G775" s="4"/>
     </row>
     <row r="776" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F776" s="4"/>
+      <c r="G776" s="4"/>
     </row>
     <row r="777" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F777" s="4"/>
+      <c r="G777" s="4"/>
     </row>
     <row r="778" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F778" s="4"/>
+      <c r="G778" s="4"/>
     </row>
     <row r="779" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F779" s="4"/>
+      <c r="G779" s="4"/>
     </row>
     <row r="780" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F780" s="4"/>
+      <c r="G780" s="4"/>
     </row>
     <row r="781" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F781" s="4"/>
+      <c r="G781" s="4"/>
     </row>
     <row r="782" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F782" s="4"/>
+      <c r="G782" s="4"/>
     </row>
     <row r="783" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F783" s="4"/>
+      <c r="G783" s="4"/>
     </row>
     <row r="784" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F784" s="4"/>
+      <c r="G784" s="4"/>
     </row>
     <row r="785" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F785" s="4"/>
+      <c r="G785" s="4"/>
     </row>
     <row r="786" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F786" s="4"/>
+      <c r="G786" s="4"/>
     </row>
     <row r="787" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F787" s="4"/>
+      <c r="G787" s="4"/>
     </row>
     <row r="788" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F788" s="4"/>
+      <c r="G788" s="4"/>
     </row>
     <row r="789" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F789" s="4"/>
+      <c r="G789" s="4"/>
     </row>
     <row r="790" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F790" s="4"/>
+      <c r="G790" s="4"/>
     </row>
     <row r="791" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F791" s="4"/>
+      <c r="G791" s="4"/>
     </row>
     <row r="792" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F792" s="4"/>
+      <c r="G792" s="4"/>
     </row>
     <row r="793" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F793" s="4"/>
+      <c r="G793" s="4"/>
     </row>
     <row r="794" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F794" s="4"/>
+      <c r="G794" s="4"/>
     </row>
     <row r="795" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F795" s="4"/>
+      <c r="G795" s="4"/>
     </row>
     <row r="796" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F796" s="4"/>
+      <c r="G796" s="4"/>
     </row>
     <row r="797" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F797" s="4"/>
+      <c r="G797" s="4"/>
     </row>
     <row r="798" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F798" s="4"/>
+      <c r="G798" s="4"/>
     </row>
     <row r="799" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F799" s="4"/>
+      <c r="G799" s="4"/>
     </row>
     <row r="800" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F800" s="4"/>
+      <c r="G800" s="4"/>
     </row>
     <row r="801" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F801" s="4"/>
+      <c r="G801" s="4"/>
     </row>
     <row r="802" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F802" s="4"/>
+      <c r="G802" s="4"/>
     </row>
     <row r="803" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F803" s="4"/>
+      <c r="G803" s="4"/>
     </row>
     <row r="804" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F804" s="4"/>
+      <c r="G804" s="4"/>
     </row>
     <row r="805" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F805" s="4"/>
+      <c r="G805" s="4"/>
     </row>
     <row r="806" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F806" s="4"/>
+      <c r="G806" s="4"/>
     </row>
     <row r="807" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F807" s="4"/>
+      <c r="G807" s="4"/>
     </row>
     <row r="808" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F808" s="4"/>
+      <c r="G808" s="4"/>
     </row>
     <row r="809" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F809" s="4"/>
+      <c r="G809" s="4"/>
     </row>
     <row r="810" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F810" s="4"/>
+      <c r="G810" s="4"/>
     </row>
     <row r="811" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F811" s="4"/>
+      <c r="G811" s="4"/>
     </row>
     <row r="812" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F812" s="4"/>
+      <c r="G812" s="4"/>
     </row>
     <row r="813" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F813" s="4"/>
+      <c r="G813" s="4"/>
     </row>
     <row r="814" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F814" s="4"/>
+      <c r="G814" s="4"/>
     </row>
     <row r="815" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F815" s="4"/>
+      <c r="G815" s="4"/>
     </row>
     <row r="816" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F816" s="4"/>
+      <c r="G816" s="4"/>
     </row>
     <row r="817" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F817" s="4"/>
+      <c r="G817" s="4"/>
     </row>
     <row r="818" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F818" s="4"/>
+      <c r="G818" s="4"/>
     </row>
     <row r="819" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F819" s="4"/>
+      <c r="G819" s="4"/>
     </row>
     <row r="820" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F820" s="4"/>
+      <c r="G820" s="4"/>
     </row>
     <row r="821" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F821" s="4"/>
+      <c r="G821" s="4"/>
     </row>
     <row r="822" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F822" s="4"/>
+      <c r="G822" s="4"/>
     </row>
     <row r="823" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F823" s="4"/>
+      <c r="G823" s="4"/>
     </row>
     <row r="824" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F824" s="4"/>
+      <c r="G824" s="4"/>
     </row>
     <row r="825" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F825" s="4"/>
+      <c r="G825" s="4"/>
     </row>
     <row r="826" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F826" s="4"/>
+      <c r="G826" s="4"/>
     </row>
     <row r="827" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F827" s="4"/>
+      <c r="G827" s="4"/>
     </row>
     <row r="828" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F828" s="4"/>
+      <c r="G828" s="4"/>
     </row>
     <row r="829" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F829" s="4"/>
+      <c r="G829" s="4"/>
     </row>
     <row r="830" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F830" s="4"/>
+      <c r="G830" s="4"/>
     </row>
     <row r="831" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F831" s="4"/>
+      <c r="G831" s="4"/>
     </row>
     <row r="832" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F832" s="4"/>
+      <c r="G832" s="4"/>
     </row>
     <row r="833" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F833" s="4"/>
+      <c r="G833" s="4"/>
     </row>
     <row r="834" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F834" s="4"/>
+      <c r="G834" s="4"/>
     </row>
     <row r="835" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F835" s="4"/>
+      <c r="G835" s="4"/>
     </row>
     <row r="836" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F836" s="4"/>
+      <c r="G836" s="4"/>
     </row>
     <row r="837" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F837" s="4"/>
+      <c r="G837" s="4"/>
     </row>
     <row r="838" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F838" s="4"/>
+      <c r="G838" s="4"/>
     </row>
     <row r="839" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F839" s="4"/>
+      <c r="G839" s="4"/>
     </row>
     <row r="840" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F840" s="4"/>
+      <c r="G840" s="4"/>
     </row>
     <row r="841" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F841" s="4"/>
+      <c r="G841" s="4"/>
     </row>
     <row r="842" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F842" s="4"/>
+      <c r="G842" s="4"/>
     </row>
     <row r="843" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F843" s="4"/>
+      <c r="G843" s="4"/>
     </row>
     <row r="844" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F844" s="4"/>
+      <c r="G844" s="4"/>
     </row>
     <row r="845" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F845" s="4"/>
+      <c r="G845" s="4"/>
     </row>
     <row r="846" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F846" s="4"/>
+      <c r="G846" s="4"/>
     </row>
     <row r="847" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F847" s="4"/>
+      <c r="G847" s="4"/>
     </row>
     <row r="848" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F848" s="4"/>
+      <c r="G848" s="4"/>
     </row>
     <row r="849" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F849" s="4"/>
+      <c r="G849" s="4"/>
     </row>
     <row r="850" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F850" s="4"/>
+      <c r="G850" s="4"/>
     </row>
     <row r="851" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F851" s="4"/>
+      <c r="G851" s="4"/>
     </row>
     <row r="852" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F852" s="4"/>
+      <c r="G852" s="4"/>
     </row>
     <row r="853" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F853" s="4"/>
+      <c r="G853" s="4"/>
     </row>
     <row r="854" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F854" s="4"/>
+      <c r="G854" s="4"/>
     </row>
     <row r="855" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F855" s="4"/>
+      <c r="G855" s="4"/>
     </row>
     <row r="856" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F856" s="4"/>
+      <c r="G856" s="4"/>
     </row>
     <row r="857" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F857" s="4"/>
+      <c r="G857" s="4"/>
     </row>
     <row r="858" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F858" s="4"/>
+      <c r="G858" s="4"/>
     </row>
     <row r="859" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F859" s="4"/>
+      <c r="G859" s="4"/>
     </row>
     <row r="860" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F860" s="4"/>
+      <c r="G860" s="4"/>
     </row>
     <row r="861" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F861" s="4"/>
+      <c r="G861" s="4"/>
     </row>
     <row r="862" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F862" s="4"/>
+      <c r="G862" s="4"/>
     </row>
     <row r="863" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F863" s="4"/>
+      <c r="G863" s="4"/>
     </row>
     <row r="864" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F864" s="4"/>
+      <c r="G864" s="4"/>
     </row>
     <row r="865" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F865" s="4"/>
+      <c r="G865" s="4"/>
     </row>
     <row r="866" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F866" s="4"/>
+      <c r="G866" s="4"/>
     </row>
     <row r="867" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F867" s="4"/>
+      <c r="G867" s="4"/>
     </row>
     <row r="868" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F868" s="4"/>
+      <c r="G868" s="4"/>
     </row>
     <row r="869" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F869" s="4"/>
+      <c r="G869" s="4"/>
     </row>
     <row r="870" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F870" s="4"/>
+      <c r="G870" s="4"/>
     </row>
     <row r="871" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F871" s="4"/>
+      <c r="G871" s="4"/>
     </row>
     <row r="872" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F872" s="4"/>
+      <c r="G872" s="4"/>
     </row>
     <row r="873" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F873" s="4"/>
+      <c r="G873" s="4"/>
     </row>
     <row r="874" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F874" s="4"/>
+      <c r="G874" s="4"/>
     </row>
     <row r="875" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F875" s="4"/>
+      <c r="G875" s="4"/>
     </row>
     <row r="876" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F876" s="4"/>
+      <c r="G876" s="4"/>
     </row>
     <row r="877" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F877" s="4"/>
+      <c r="G877" s="4"/>
     </row>
     <row r="878" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F878" s="4"/>
+      <c r="G878" s="4"/>
     </row>
     <row r="879" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F879" s="4"/>
+      <c r="G879" s="4"/>
     </row>
     <row r="880" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F880" s="4"/>
+      <c r="G880" s="4"/>
     </row>
     <row r="881" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F881" s="4"/>
+      <c r="G881" s="4"/>
     </row>
     <row r="882" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F882" s="4"/>
+      <c r="G882" s="4"/>
     </row>
     <row r="883" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F883" s="4"/>
+      <c r="G883" s="4"/>
     </row>
     <row r="884" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F884" s="4"/>
+      <c r="G884" s="4"/>
     </row>
     <row r="885" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F885" s="4"/>
+      <c r="G885" s="4"/>
     </row>
     <row r="886" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F886" s="4"/>
+      <c r="G886" s="4"/>
     </row>
     <row r="887" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F887" s="4"/>
+      <c r="G887" s="4"/>
     </row>
     <row r="888" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F888" s="4"/>
+      <c r="G888" s="4"/>
     </row>
     <row r="889" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F889" s="4"/>
+      <c r="G889" s="4"/>
     </row>
     <row r="890" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F890" s="4"/>
+      <c r="G890" s="4"/>
     </row>
     <row r="891" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F891" s="4"/>
+      <c r="G891" s="4"/>
     </row>
     <row r="892" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F892" s="4"/>
+      <c r="G892" s="4"/>
     </row>
     <row r="893" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F893" s="4"/>
+      <c r="G893" s="4"/>
     </row>
     <row r="894" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F894" s="4"/>
+      <c r="G894" s="4"/>
     </row>
     <row r="895" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F895" s="4"/>
+      <c r="G895" s="4"/>
     </row>
     <row r="896" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F896" s="4"/>
+      <c r="G896" s="4"/>
     </row>
     <row r="897" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F897" s="4"/>
+      <c r="G897" s="4"/>
     </row>
     <row r="898" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F898" s="4"/>
+      <c r="G898" s="4"/>
     </row>
     <row r="899" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F899" s="4"/>
+      <c r="G899" s="4"/>
     </row>
     <row r="900" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F900" s="4"/>
+      <c r="G900" s="4"/>
     </row>
     <row r="901" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F901" s="4"/>
+      <c r="G901" s="4"/>
     </row>
     <row r="902" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F902" s="4"/>
+      <c r="G902" s="4"/>
     </row>
     <row r="903" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F903" s="4"/>
+      <c r="G903" s="4"/>
     </row>
     <row r="904" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F904" s="4"/>
+      <c r="G904" s="4"/>
     </row>
     <row r="905" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F905" s="4"/>
+      <c r="G905" s="4"/>
     </row>
     <row r="906" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F906" s="4"/>
+      <c r="G906" s="4"/>
     </row>
     <row r="907" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F907" s="4"/>
+      <c r="G907" s="4"/>
     </row>
     <row r="908" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F908" s="4"/>
+      <c r="G908" s="4"/>
     </row>
     <row r="909" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F909" s="4"/>
+      <c r="G909" s="4"/>
     </row>
     <row r="910" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F910" s="4"/>
+      <c r="G910" s="4"/>
     </row>
     <row r="911" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F911" s="4"/>
+      <c r="G911" s="4"/>
     </row>
     <row r="912" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F912" s="4"/>
+      <c r="G912" s="4"/>
     </row>
     <row r="913" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F913" s="4"/>
+      <c r="G913" s="4"/>
     </row>
     <row r="914" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F914" s="4"/>
+      <c r="G914" s="4"/>
     </row>
     <row r="915" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F915" s="4"/>
+      <c r="G915" s="4"/>
     </row>
     <row r="916" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F916" s="4"/>
+      <c r="G916" s="4"/>
     </row>
     <row r="917" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F917" s="4"/>
+      <c r="G917" s="4"/>
     </row>
     <row r="918" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F918" s="4"/>
+      <c r="G918" s="4"/>
     </row>
     <row r="919" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F919" s="4"/>
+      <c r="G919" s="4"/>
     </row>
     <row r="920" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F920" s="4"/>
+      <c r="G920" s="4"/>
     </row>
     <row r="921" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F921" s="4"/>
+      <c r="G921" s="4"/>
     </row>
     <row r="922" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F922" s="4"/>
+      <c r="G922" s="4"/>
     </row>
     <row r="923" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F923" s="4"/>
+      <c r="G923" s="4"/>
     </row>
     <row r="924" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F924" s="4"/>
+      <c r="G924" s="4"/>
     </row>
     <row r="925" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F925" s="4"/>
+      <c r="G925" s="4"/>
     </row>
     <row r="926" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F926" s="4"/>
+      <c r="G926" s="4"/>
     </row>
     <row r="927" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F927" s="4"/>
+      <c r="G927" s="4"/>
     </row>
     <row r="928" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F928" s="4"/>
+      <c r="G928" s="4"/>
     </row>
     <row r="929" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F929" s="4"/>
+      <c r="G929" s="4"/>
     </row>
     <row r="930" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F930" s="4"/>
+      <c r="G930" s="4"/>
     </row>
     <row r="931" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F931" s="4"/>
+      <c r="G931" s="4"/>
     </row>
     <row r="932" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F932" s="4"/>
+      <c r="G932" s="4"/>
     </row>
     <row r="933" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F933" s="4"/>
+      <c r="G933" s="4"/>
     </row>
     <row r="934" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F934" s="4"/>
+      <c r="G934" s="4"/>
     </row>
     <row r="935" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F935" s="4"/>
+      <c r="G935" s="4"/>
     </row>
     <row r="936" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F936" s="4"/>
+      <c r="G936" s="4"/>
     </row>
     <row r="937" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F937" s="4"/>
+      <c r="G937" s="4"/>
     </row>
     <row r="938" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F938" s="4"/>
+      <c r="G938" s="4"/>
     </row>
     <row r="939" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F939" s="4"/>
+      <c r="G939" s="4"/>
     </row>
     <row r="940" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F940" s="4"/>
+      <c r="G940" s="4"/>
     </row>
     <row r="941" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F941" s="4"/>
+      <c r="G941" s="4"/>
     </row>
     <row r="942" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F942" s="4"/>
+      <c r="G942" s="4"/>
     </row>
     <row r="943" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F943" s="4"/>
+      <c r="G943" s="4"/>
     </row>
     <row r="944" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F944" s="4"/>
+      <c r="G944" s="4"/>
     </row>
     <row r="945" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F945" s="4"/>
+      <c r="G945" s="4"/>
     </row>
     <row r="946" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F946" s="4"/>
+      <c r="G946" s="4"/>
     </row>
     <row r="947" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F947" s="4"/>
+      <c r="G947" s="4"/>
     </row>
     <row r="948" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F948" s="4"/>
+      <c r="G948" s="4"/>
     </row>
     <row r="949" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F949" s="4"/>
+      <c r="G949" s="4"/>
     </row>
     <row r="950" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F950" s="4"/>
+      <c r="G950" s="4"/>
     </row>
     <row r="951" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F951" s="4"/>
+      <c r="G951" s="4"/>
     </row>
     <row r="952" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F952" s="4"/>
+      <c r="G952" s="4"/>
     </row>
     <row r="953" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F953" s="4"/>
+      <c r="G953" s="4"/>
     </row>
     <row r="954" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F954" s="4"/>
+      <c r="G954" s="4"/>
     </row>
     <row r="955" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F955" s="4"/>
+      <c r="G955" s="4"/>
     </row>
     <row r="956" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F956" s="4"/>
+      <c r="G956" s="4"/>
     </row>
     <row r="957" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F957" s="4"/>
+      <c r="G957" s="4"/>
     </row>
     <row r="958" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F958" s="4"/>
+      <c r="G958" s="4"/>
     </row>
     <row r="959" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F959" s="4"/>
+      <c r="G959" s="4"/>
     </row>
     <row r="960" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F960" s="4"/>
+      <c r="G960" s="4"/>
     </row>
     <row r="961" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F961" s="4"/>
+      <c r="G961" s="4"/>
     </row>
     <row r="962" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F962" s="4"/>
+      <c r="G962" s="4"/>
     </row>
     <row r="963" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F963" s="4"/>
+      <c r="G963" s="4"/>
     </row>
     <row r="964" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F964" s="4"/>
+      <c r="G964" s="4"/>
     </row>
     <row r="965" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F965" s="4"/>
+      <c r="G965" s="4"/>
     </row>
     <row r="966" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F966" s="4"/>
+      <c r="G966" s="4"/>
     </row>
     <row r="967" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F967" s="4"/>
+      <c r="G967" s="4"/>
     </row>
     <row r="968" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F968" s="4"/>
+      <c r="G968" s="4"/>
     </row>
     <row r="969" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F969" s="4"/>
+      <c r="G969" s="4"/>
     </row>
     <row r="970" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F970" s="4"/>
+      <c r="G970" s="4"/>
     </row>
     <row r="971" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F971" s="4"/>
+      <c r="G971" s="4"/>
     </row>
     <row r="972" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F972" s="4"/>
+      <c r="G972" s="4"/>
     </row>
     <row r="973" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F973" s="4"/>
+      <c r="G973" s="4"/>
     </row>
     <row r="974" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F974" s="4"/>
+      <c r="G974" s="4"/>
     </row>
     <row r="975" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F975" s="4"/>
+      <c r="G975" s="4"/>
     </row>
     <row r="976" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F976" s="4"/>
+      <c r="G976" s="4"/>
     </row>
     <row r="977" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F977" s="4"/>
+      <c r="G977" s="4"/>
     </row>
     <row r="978" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F978" s="4"/>
+      <c r="G978" s="4"/>
     </row>
     <row r="979" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F979" s="4"/>
+      <c r="G979" s="4"/>
     </row>
     <row r="980" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F980" s="4"/>
+      <c r="G980" s="4"/>
     </row>
     <row r="981" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F981" s="4"/>
+      <c r="G981" s="4"/>
     </row>
     <row r="982" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F982" s="4"/>
+      <c r="G982" s="4"/>
     </row>
     <row r="983" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F983" s="4"/>
+      <c r="G983" s="4"/>
     </row>
     <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F984" s="4"/>
+      <c r="G984" s="4"/>
     </row>
     <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F985" s="4"/>
+      <c r="G985" s="4"/>
     </row>
     <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F986" s="4"/>
+      <c r="G986" s="4"/>
     </row>
     <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F987" s="4"/>
+      <c r="G987" s="4"/>
     </row>
     <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F988" s="4"/>
+      <c r="G988" s="4"/>
     </row>
     <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F989" s="4"/>
+      <c r="G989" s="4"/>
     </row>
     <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F990" s="4"/>
+      <c r="G990" s="4"/>
     </row>
     <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F991" s="4"/>
+      <c r="G991" s="4"/>
     </row>
     <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F992" s="4"/>
+      <c r="G992" s="4"/>
     </row>
     <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F993" s="4"/>
+      <c r="G993" s="4"/>
     </row>
     <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F994" s="4"/>
+      <c r="G994" s="4"/>
     </row>
     <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F995" s="4"/>
+      <c r="G995" s="4"/>
     </row>
     <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F996" s="4"/>
+      <c r="G996" s="4"/>
     </row>
     <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F997" s="4"/>
+      <c r="G997" s="4"/>
     </row>
     <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F998" s="4"/>
+      <c r="G998" s="4"/>
     </row>
     <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
     </row>
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F1000" s="4"/>
+      <c r="G1000" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2" type="list">
       <formula1>'Giải thích nguồn tìm kiếm'!$A$1:$A$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3337,7 +3350,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.76"/>
@@ -3345,90 +3358,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>